<commit_message>
updated the state dataset
</commit_message>
<xml_diff>
--- a/data/StateCOVID-19.xlsx
+++ b/data/StateCOVID-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anish.walia/Documents/My Projects/COVID-19-INDIA-TRACKER/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23EDCE7-B1E0-CC46-B552-42C8F477E7B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688F2946-D54D-9649-8B6F-186474B0654E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="15520" xr2:uid="{A0CBF040-3DE4-F64D-A276-2E742F59E5E8}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -216,22 +216,15 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -261,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -269,10 +262,9 @@
     <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,28 +582,25 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="10.83203125" style="8"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1"/>
@@ -624,21 +613,22 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>4917</v>
+        <v>6653</v>
       </c>
       <c r="C2" s="3">
-        <v>386</v>
+        <v>602</v>
       </c>
       <c r="D2" s="3">
-        <v>136</v>
+        <v>209</v>
       </c>
       <c r="E2" s="3">
-        <v>4395</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+        <v>5842</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -646,49 +636,49 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-    </row>
-    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>891</v>
+        <v>1346</v>
       </c>
       <c r="C4" s="5">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="D4" s="5">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="E4" s="3">
-        <v>769</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+        <v>1148</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="5">
-        <v>621</v>
+        <v>834</v>
       </c>
       <c r="C5" s="5">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3">
-        <v>603</v>
+        <v>799</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="6"/>
@@ -701,16 +691,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="5">
-        <v>525</v>
+        <v>720</v>
       </c>
       <c r="C6" s="5">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
-        <v>502</v>
+        <v>683</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="6"/>
@@ -720,19 +710,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5">
-        <v>327</v>
-      </c>
-      <c r="C7" s="5">
-        <v>59</v>
+        <v>471</v>
+      </c>
+      <c r="C7" s="6">
+        <v>45</v>
       </c>
       <c r="D7" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3">
-        <v>266</v>
+        <v>415</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="6"/>
@@ -742,19 +732,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5">
-        <v>364</v>
+        <v>430</v>
       </c>
       <c r="C8" s="6">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D8" s="5">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>320</v>
+        <v>382</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="6"/>
@@ -764,19 +754,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5">
-        <v>305</v>
-      </c>
-      <c r="C9" s="6">
-        <v>21</v>
+        <v>357</v>
+      </c>
+      <c r="C9" s="5">
+        <v>97</v>
       </c>
       <c r="D9" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="6"/>
@@ -786,19 +776,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="5">
-        <v>325</v>
+        <v>410</v>
       </c>
       <c r="C10" s="6">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10" s="3">
-        <v>298</v>
+        <v>375</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="6"/>
@@ -811,16 +801,16 @@
         <v>18</v>
       </c>
       <c r="B11" s="5">
-        <v>304</v>
+        <v>363</v>
       </c>
       <c r="C11" s="5">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
         <v>5</v>
       </c>
-      <c r="D11" s="5">
-        <v>3</v>
-      </c>
       <c r="E11" s="3">
-        <v>296</v>
+        <v>348</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="6"/>
@@ -833,16 +823,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="5">
-        <v>268</v>
+        <v>397</v>
       </c>
       <c r="C12" s="5">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E12" s="3">
-        <v>239</v>
+        <v>339</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="6"/>
@@ -855,16 +845,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="5">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="C13" s="5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E13" s="3">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="6"/>
@@ -877,16 +867,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="5">
-        <v>165</v>
+        <v>262</v>
       </c>
       <c r="C14" s="6">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E14" s="3">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="6"/>
@@ -896,19 +886,19 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" s="5">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="C15" s="5">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D15" s="5">
         <v>2</v>
       </c>
       <c r="E15" s="3">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="6"/>
@@ -918,19 +908,19 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="C16" s="5">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D16" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="3">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="6"/>
@@ -943,16 +933,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="5">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="C17" s="5">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D17" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E17" s="3">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="6"/>
@@ -965,16 +955,16 @@
         <v>19</v>
       </c>
       <c r="B18" s="5">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C18" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D18" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E18" s="3">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="6"/>
@@ -984,19 +974,19 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B19" s="5">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C19" s="5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
       </c>
       <c r="E19" s="3">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="6"/>
@@ -1006,19 +996,19 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C20" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="6"/>
@@ -1031,16 +1021,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="5">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C21" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" s="5">
         <v>0</v>
       </c>
       <c r="E21" s="3">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="6"/>
@@ -1050,19 +1040,19 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B22" s="5">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C22" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="5">
         <v>0</v>
       </c>
       <c r="E22" s="3">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="6"/>
@@ -1078,13 +1068,13 @@
         <v>18</v>
       </c>
       <c r="C23" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D23" s="5">
         <v>0</v>
       </c>
       <c r="E23" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="6"/>
@@ -1094,19 +1084,19 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B24" s="5">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C24" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="3">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="6"/>
@@ -1116,19 +1106,19 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5">
         <v>10</v>
       </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
       <c r="D25" s="5">
         <v>0</v>
       </c>
       <c r="E25" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
@@ -1138,19 +1128,19 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D26" s="5">
         <v>0</v>
       </c>
       <c r="E26" s="3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="6"/>
@@ -1160,19 +1150,19 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="5">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C27" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D27" s="5">
         <v>0</v>
       </c>
       <c r="E27" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="6"/>
@@ -1182,19 +1172,19 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28" s="3">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="6"/>
@@ -1210,13 +1200,13 @@
         <v>5</v>
       </c>
       <c r="C29" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="5">
         <v>0</v>
       </c>
       <c r="E29" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="6"/>
@@ -1229,16 +1219,16 @@
         <v>36</v>
       </c>
       <c r="B30" s="5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C30" s="5">
         <v>0</v>
       </c>
       <c r="D30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="3">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="6"/>
@@ -1336,10 +1326,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B35" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="5">
         <v>0</v>
@@ -1348,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="6"/>
@@ -1358,7 +1348,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5">
         <v>0</v>
@@ -1380,7 +1370,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="5">
         <v>0</v>
@@ -1402,7 +1392,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="5">
         <v>0</v>
@@ -1424,7 +1414,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
@@ -1446,10 +1436,10 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" s="5">
         <v>0</v>
@@ -1458,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="6"/>

</xml_diff>

<commit_message>
updated the state data
</commit_message>
<xml_diff>
--- a/data/StateCOVID-19.xlsx
+++ b/data/StateCOVID-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anish.walia/Documents/My Projects/COVID-19-INDIA-TRACKER/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688F2946-D54D-9649-8B6F-186474B0654E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF6FD30-18D6-9649-AF8E-7387329E102C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="15520" xr2:uid="{A0CBF040-3DE4-F64D-A276-2E742F59E5E8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Confirmed</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Last_Updated_Time</t>
   </si>
   <si>
     <t>Total</t>
@@ -168,7 +171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -221,25 +224,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="13"/>
-      <color theme="0"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,9 +253,7 @@
     <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,103 +571,96 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>6653</v>
-      </c>
-      <c r="C2" s="3">
-        <v>602</v>
-      </c>
-      <c r="D2" s="3">
-        <v>209</v>
-      </c>
-      <c r="E2" s="3">
-        <v>5842</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5">
-        <v>1346</v>
-      </c>
-      <c r="C4" s="5">
-        <v>117</v>
-      </c>
-      <c r="D4" s="5">
-        <v>81</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1148</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="B3" s="3">
+        <v>6910</v>
+      </c>
+      <c r="C3" s="3">
+        <v>642</v>
+      </c>
+      <c r="D3" s="3">
+        <v>230</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6038</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5">
-        <v>834</v>
+        <v>1364</v>
       </c>
       <c r="C5" s="5">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="D5" s="5">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="E5" s="3">
-        <v>799</v>
+        <v>1141</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="6"/>
@@ -688,19 +670,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5">
-        <v>720</v>
+        <v>834</v>
       </c>
       <c r="C6" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3">
-        <v>683</v>
+        <v>799</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="6"/>
@@ -710,19 +692,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5">
-        <v>471</v>
-      </c>
-      <c r="C7" s="6">
-        <v>45</v>
+        <v>720</v>
+      </c>
+      <c r="C7" s="5">
+        <v>25</v>
       </c>
       <c r="D7" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3">
-        <v>415</v>
+        <v>683</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="6"/>
@@ -732,19 +714,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="5">
-        <v>430</v>
+        <v>471</v>
       </c>
       <c r="C8" s="6">
         <v>45</v>
       </c>
       <c r="D8" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="6"/>
@@ -754,19 +736,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5">
-        <v>357</v>
-      </c>
-      <c r="C9" s="5">
-        <v>97</v>
+        <v>520</v>
+      </c>
+      <c r="C9" s="6">
+        <v>60</v>
       </c>
       <c r="D9" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="3">
-        <v>258</v>
+        <v>457</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="6"/>
@@ -776,19 +758,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5">
-        <v>410</v>
-      </c>
-      <c r="C10" s="6">
-        <v>31</v>
+        <v>357</v>
+      </c>
+      <c r="C10" s="5">
+        <v>97</v>
       </c>
       <c r="D10" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3">
-        <v>375</v>
+        <v>258</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="6"/>
@@ -798,19 +780,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5">
-        <v>363</v>
-      </c>
-      <c r="C11" s="5">
-        <v>10</v>
+        <v>431</v>
+      </c>
+      <c r="C11" s="6">
+        <v>32</v>
       </c>
       <c r="D11" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="3">
-        <v>348</v>
+        <v>395</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="6"/>
@@ -820,19 +802,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5">
-        <v>397</v>
+        <v>365</v>
       </c>
       <c r="C12" s="5">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D12" s="5">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="6"/>
@@ -842,19 +824,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5">
-        <v>197</v>
+        <v>411</v>
       </c>
       <c r="C13" s="5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E13" s="3">
-        <v>161</v>
+        <v>353</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="6"/>
@@ -864,19 +846,19 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>262</v>
-      </c>
-      <c r="C14" s="6">
-        <v>26</v>
+        <v>207</v>
+      </c>
+      <c r="C14" s="5">
+        <v>30</v>
       </c>
       <c r="D14" s="5">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E14" s="3">
-        <v>218</v>
+        <v>171</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="6"/>
@@ -886,19 +868,19 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>170</v>
-      </c>
-      <c r="C15" s="5">
-        <v>32</v>
+        <v>308</v>
+      </c>
+      <c r="C15" s="6">
+        <v>30</v>
       </c>
       <c r="D15" s="5">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E15" s="3">
-        <v>136</v>
+        <v>259</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="6"/>
@@ -908,19 +890,19 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C16" s="5">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="3">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="6"/>
@@ -930,19 +912,19 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>130</v>
+        <v>207</v>
       </c>
       <c r="C17" s="5">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D17" s="5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E17" s="3">
-        <v>102</v>
+        <v>197</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="6"/>
@@ -952,19 +934,19 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="C18" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D18" s="5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="6"/>
@@ -974,19 +956,19 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="C19" s="5">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D19" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E19" s="3">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="6"/>
@@ -996,19 +978,19 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B20" s="5">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C20" s="5">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="6"/>
@@ -1018,19 +1000,19 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C21" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="6"/>
@@ -1040,19 +1022,19 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C22" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D22" s="5">
         <v>0</v>
       </c>
       <c r="E22" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="6"/>
@@ -1062,19 +1044,19 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B23" s="5">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C23" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="3">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="6"/>
@@ -1084,19 +1066,19 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C24" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D24" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24" s="3">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="6"/>
@@ -1106,19 +1088,19 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B25" s="5">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C25" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D25" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" s="3">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
@@ -1128,19 +1110,19 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="5">
+        <v>15</v>
+      </c>
+      <c r="C26" s="5">
         <v>11</v>
       </c>
-      <c r="C26" s="5">
-        <v>0</v>
-      </c>
       <c r="D26" s="5">
         <v>0</v>
       </c>
       <c r="E26" s="3">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="6"/>
@@ -1153,16 +1135,16 @@
         <v>24</v>
       </c>
       <c r="B27" s="5">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C27" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" s="5">
         <v>0</v>
       </c>
       <c r="E27" s="3">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="6"/>
@@ -1172,19 +1154,19 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="5">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C28" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D28" s="5">
         <v>0</v>
       </c>
       <c r="E28" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="6"/>
@@ -1194,10 +1176,10 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B29" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C29" s="5">
         <v>1</v>
@@ -1206,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="6"/>
@@ -1216,19 +1198,19 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B30" s="5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="6"/>
@@ -1238,19 +1220,19 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B31" s="5">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C31" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="6"/>
@@ -1263,10 +1245,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="5">
         <v>0</v>
@@ -1282,7 +1264,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
@@ -1304,7 +1286,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="5">
         <v>1</v>
@@ -1326,7 +1308,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -1348,10 +1330,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B36" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="5">
         <v>0</v>
@@ -1360,7 +1342,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="6"/>
@@ -1370,7 +1352,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5">
         <v>0</v>
@@ -1457,11 +1439,25 @@
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
       <c r="H41" s="4"/>
       <c r="I41" s="6"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the dataset with latest data
</commit_message>
<xml_diff>
--- a/data/StateCOVID-19.xlsx
+++ b/data/StateCOVID-19.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anish.walia/Documents/My Projects/COVID-19-INDIA-TRACKER/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BFC7E6-3AFC-8941-873A-B6311B28632E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAA16FE-3278-F041-AC00-B04893CACBE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="15520" xr2:uid="{A0CBF040-3DE4-F64D-A276-2E742F59E5E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,16 +618,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>11511</v>
+        <v>12321</v>
       </c>
       <c r="C3" s="3">
-        <v>1366</v>
+        <v>1498</v>
       </c>
       <c r="D3" s="3">
-        <v>394</v>
+        <v>420</v>
       </c>
       <c r="E3" s="3">
-        <v>9751</v>
+        <v>10403</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="6"/>
@@ -654,16 +654,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="5">
-        <v>2684</v>
+        <v>2916</v>
       </c>
       <c r="C5" s="5">
-        <v>259</v>
+        <v>295</v>
       </c>
       <c r="D5" s="5">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E5" s="3">
-        <v>2247</v>
+        <v>2434</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="6"/>
@@ -700,16 +700,16 @@
         <v>14</v>
       </c>
       <c r="B7" s="5">
-        <v>1204</v>
+        <v>1242</v>
       </c>
       <c r="C7" s="5">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="D7" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="6"/>
@@ -723,7 +723,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="5">
-        <v>1005</v>
+        <v>1046</v>
       </c>
       <c r="C8" s="6">
         <v>147</v>
@@ -732,7 +732,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="3">
-        <v>847</v>
+        <v>888</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="6"/>
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="5">
-        <v>741</v>
+        <v>938</v>
       </c>
       <c r="C9" s="5">
         <v>64</v>
@@ -755,7 +755,7 @@
         <v>53</v>
       </c>
       <c r="E9" s="3">
-        <v>624</v>
+        <v>821</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="6"/>
@@ -769,16 +769,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>660</v>
+        <v>735</v>
       </c>
       <c r="C10" s="6">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D10" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3">
-        <v>602</v>
+        <v>667</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="6"/>
@@ -792,16 +792,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="5">
-        <v>650</v>
+        <v>766</v>
       </c>
       <c r="C11" s="6">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D11" s="5">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E11" s="3">
-        <v>563</v>
+        <v>669</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="6"/>
@@ -815,16 +815,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="5">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="C12" s="6">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D12" s="5">
         <v>18</v>
       </c>
       <c r="E12" s="3">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="6"/>
@@ -838,16 +838,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="5">
-        <v>483</v>
+        <v>525</v>
       </c>
       <c r="C13" s="5">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3">
-        <v>458</v>
+        <v>491</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="6"/>
@@ -861,16 +861,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="5">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C14" s="5">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D14" s="5">
         <v>2</v>
       </c>
       <c r="E14" s="3">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="6"/>
@@ -884,16 +884,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="5">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="C15" s="5">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D15" s="5">
         <v>4</v>
       </c>
       <c r="E15" s="3">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="6"/>
@@ -907,16 +907,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="5">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="C16" s="5">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D16" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="3">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="6"/>
@@ -930,16 +930,16 @@
         <v>18</v>
       </c>
       <c r="B17" s="5">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C17" s="5">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17" s="5">
         <v>3</v>
       </c>
       <c r="E17" s="3">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="6"/>
@@ -976,7 +976,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="5">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C19" s="5">
         <v>27</v>
@@ -985,7 +985,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="3">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="6"/>
@@ -999,7 +999,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="5">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C20" s="5">
         <v>29</v>
@@ -1008,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="6"/>
@@ -1071,13 +1071,13 @@
         <v>33</v>
       </c>
       <c r="C23" s="5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D23" s="5">
         <v>0</v>
       </c>
       <c r="E23" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="6"/>
@@ -1091,7 +1091,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="5">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5">
         <v>13</v>
@@ -1100,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="6"/>
@@ -1117,13 +1117,13 @@
         <v>32</v>
       </c>
       <c r="C25" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
       <c r="E25" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
@@ -1137,7 +1137,7 @@
         <v>37</v>
       </c>
       <c r="B26" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="5">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="6"/>
@@ -1163,13 +1163,13 @@
         <v>21</v>
       </c>
       <c r="C27" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D27" s="5">
         <v>0</v>
       </c>
       <c r="E27" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="6"/>
@@ -1232,13 +1232,13 @@
         <v>7</v>
       </c>
       <c r="C30" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D30" s="5">
         <v>0</v>
       </c>
       <c r="E30" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="6"/>
@@ -1301,13 +1301,13 @@
         <v>2</v>
       </c>
       <c r="C33" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="5">
         <v>0</v>
       </c>
       <c r="E33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="6"/>
@@ -1347,13 +1347,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="5">
         <v>0</v>
       </c>
       <c r="E35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="6"/>
@@ -1413,7 +1413,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C38" s="5">
         <v>0</v>
@@ -1422,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="6"/>

</xml_diff>